<commit_message>
Change column name in excel
Change column name in laboratory excel

Envoyé depuis mon iPhone.
P.S. : Ce commit est certifié sans gluten
</commit_message>
<xml_diff>
--- a/tests/resources/integration_annonce_laboratoire.xlsx
+++ b/tests/resources/integration_annonce_laboratoire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerylcdp/PycharmProjects/importApp/tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE04B4C-E545-E747-A1B6-214BD65009AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86089E7-6A01-2C4F-8C1A-A3E08A9D0845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,9 +169,6 @@
     <t>CIP/ACL ou EAN*</t>
   </si>
   <si>
-    <t>Désignation - Nom du produit*</t>
-  </si>
-  <si>
     <t>Vendu par (nombre) - colisage*</t>
   </si>
   <si>
@@ -324,9 +321,6 @@
 - 0%</t>
   </si>
   <si>
-    <t>PU HT catalogue*</t>
-  </si>
-  <si>
     <t>Par quelle quantité vous souhaitez vendre 1 référence produit.</t>
   </si>
   <si>
@@ -337,9 +331,6 @@
 - unitaire
 - palier
 - devis</t>
-  </si>
-  <si>
-    <t>Unité gratuite</t>
   </si>
   <si>
     <t>Uniquement pour les produits distribué par palier</t>
@@ -501,6 +492,15 @@
   </si>
   <si>
     <t xml:space="preserve"> My DCI</t>
+  </si>
+  <si>
+    <t>Désignation - Nom du produit***</t>
+  </si>
+  <si>
+    <t>Unité gratuite</t>
+  </si>
+  <si>
+    <t>PU HT catalogue***</t>
   </si>
 </sst>
 </file>
@@ -1212,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E187B0-E1B1-A140-A8DF-8FBDDEEAA214}">
   <dimension ref="A1:P138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1229,7 +1229,7 @@
     <col min="10" max="10" width="37.1640625" customWidth="1"/>
     <col min="11" max="11" width="45.33203125" customWidth="1"/>
     <col min="12" max="12" width="38.6640625" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" customWidth="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.33203125" style="27" bestFit="1" customWidth="1"/>
   </cols>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="2" spans="1:16" ht="154" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1266,7 +1266,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="1"/>
       <c r="J2" s="26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1276,97 +1276,97 @@
     </row>
     <row r="3" spans="1:16" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="30" t="s">
-        <v>4</v>
-      </c>
       <c r="O3" s="34" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="P3" s="31"/>
     </row>
     <row r="4" spans="1:16" ht="91" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>6</v>
-      </c>
       <c r="D4" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>30</v>
-      </c>
       <c r="L4" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="N4" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="33" t="s">
         <v>37</v>
-      </c>
-      <c r="N4" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" s="33" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="19" customFormat="1" ht="29" x14ac:dyDescent="0.2">
@@ -1377,28 +1377,28 @@
         <v>3492270078044</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F5" s="9">
         <v>70</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5" s="11">
         <v>5.5</v>
       </c>
       <c r="I5" s="41" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K5" s="46">
         <v>20</v>
@@ -1424,28 +1424,28 @@
         <v>3492270005057</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F6" s="9">
         <v>55</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" s="11">
         <v>5.5</v>
       </c>
       <c r="I6" s="41" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K6" s="46">
         <v>6</v>
@@ -1469,28 +1469,28 @@
         <v>3492270078112</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F7" s="9">
         <v>75</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H7" s="11">
         <v>5.5</v>
       </c>
       <c r="I7" s="37" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K7" s="47">
         <v>6</v>
@@ -1514,28 +1514,28 @@
         <v>3492270078082</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F8" s="9">
         <v>520</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H8" s="9">
         <v>5.5</v>
       </c>
       <c r="I8" s="41" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K8" s="46">
         <v>6</v>
@@ -1559,28 +1559,28 @@
         <v>3492270078082</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F9" s="9">
         <v>520</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H9" s="9">
         <v>5.5</v>
       </c>
       <c r="I9" s="41" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K9" s="46">
         <v>6</v>
@@ -1604,28 +1604,28 @@
         <v>3492270078044</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F10" s="9">
         <v>70</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H10" s="11">
         <v>5.5</v>
       </c>
       <c r="I10" s="41" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K10" s="46">
         <v>10</v>
@@ -1649,28 +1649,28 @@
       </c>
       <c r="B11" s="36"/>
       <c r="C11" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F11" s="9">
         <v>370</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H11" s="9">
         <v>5.5</v>
       </c>
       <c r="I11" s="41" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K11" s="46">
         <v>6</v>
@@ -3812,36 +3812,36 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>23</v>
-      </c>
       <c r="D1" s="22" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="19">
         <v>20</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="54" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E2" s="19">
         <v>3</v>
@@ -3852,29 +3852,29 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="19">
         <v>10</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="19">
         <v>5.5</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="19">
         <v>2.1</v>
@@ -3883,7 +3883,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="19">
         <v>0</v>
@@ -3892,7 +3892,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>

</xml_diff>

<commit_message>
Add stock for laboratory
Envoyé depuis mon iPhone.
P.S. : Ce commit est certifié sans gluten
</commit_message>
<xml_diff>
--- a/tests/resources/integration_annonce_laboratoire.xlsx
+++ b/tests/resources/integration_annonce_laboratoire.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerylcdp/PycharmProjects/importApp/tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC774EB3-73A8-5E4F-B2A4-8ADBD217DE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C37FB8-2346-2342-853D-8D01AF689F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33280" yWindow="-440" windowWidth="33280" windowHeight="17020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Annonces" sheetId="1" r:id="rId1"/>
     <sheet name="Parametre" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Annonces!$A$1:$O$138</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Annonces!$A$1:$P$138</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -70,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="73">
   <si>
     <t>3/ Remplir les infos produits (pour chaque produit) :</t>
   </si>
@@ -521,6 +532,13 @@
 - disabled
 - holiday
 - archived</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Si vous possédez un stock limité veuillez indiquer le nombre d'unité à mettre en vente. 
+Sinon ne rien mettre</t>
   </si>
 </sst>
 </file>
@@ -1260,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q138"/>
+  <dimension ref="A1:R138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1277,16 +1295,16 @@
     <col min="8" max="8" width="17.5" customWidth="1"/>
     <col min="9" max="9" width="56.1640625" customWidth="1"/>
     <col min="10" max="10" width="37.1640625" customWidth="1"/>
-    <col min="11" max="11" width="45.33203125" customWidth="1"/>
-    <col min="12" max="12" width="38.6640625" customWidth="1"/>
-    <col min="13" max="13" width="17.83203125" customWidth="1"/>
-    <col min="14" max="14" width="16" customWidth="1"/>
-    <col min="15" max="15" width="20.33203125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="30.1640625" customWidth="1"/>
-    <col min="17" max="17" width="39.6640625" customWidth="1"/>
+    <col min="11" max="12" width="45.33203125" customWidth="1"/>
+    <col min="13" max="13" width="38.6640625" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" customWidth="1"/>
+    <col min="15" max="15" width="16" customWidth="1"/>
+    <col min="16" max="16" width="20.33203125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="30.1640625" customWidth="1"/>
+    <col min="18" max="18" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1295,10 +1313,11 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="5"/>
-    </row>
-    <row r="2" spans="1:17" ht="154" x14ac:dyDescent="0.15">
+      <c r="M1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="5"/>
+    </row>
+    <row r="2" spans="1:18" ht="154" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1309,10 +1328,11 @@
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="8"/>
-    </row>
-    <row r="3" spans="1:17" ht="28" x14ac:dyDescent="0.15">
+      <c r="M2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="8"/>
+    </row>
+    <row r="3" spans="1:18" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
@@ -1347,25 +1367,28 @@
         <v>13</v>
       </c>
       <c r="L3" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="M3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="N3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="O3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="P3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="Q3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="R3" s="11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="104" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" ht="104" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>19</v>
       </c>
@@ -1399,26 +1422,29 @@
       <c r="K4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="M4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="N4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="O4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="P4" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="16" t="s">
+      <c r="Q4" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="38" t="s">
+      <c r="R4" s="38" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="29" x14ac:dyDescent="0.2">
       <c r="A5" s="17">
         <v>470</v>
       </c>
@@ -1453,25 +1479,28 @@
         <v>20</v>
       </c>
       <c r="L5" s="20">
+        <v>2</v>
+      </c>
+      <c r="M5" s="20">
         <v>10</v>
       </c>
-      <c r="M5" s="24">
+      <c r="N5" s="24">
         <v>16.420000000000002</v>
       </c>
-      <c r="N5" s="25">
+      <c r="O5" s="25">
         <v>20</v>
       </c>
-      <c r="O5" s="26">
+      <c r="P5" s="26">
         <v>12</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>41</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="43" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="43" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
         <v>500</v>
       </c>
@@ -1505,24 +1534,27 @@
       <c r="K6" s="20">
         <v>6</v>
       </c>
-      <c r="L6" s="20"/>
-      <c r="M6" s="24">
+      <c r="L6" s="20">
+        <v>3</v>
+      </c>
+      <c r="M6" s="20"/>
+      <c r="N6" s="24">
         <v>9.84</v>
       </c>
-      <c r="N6" s="25">
+      <c r="O6" s="25">
         <v>7.38</v>
       </c>
-      <c r="O6" s="26">
+      <c r="P6" s="26">
         <v>12</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>46</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="43" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="43" x14ac:dyDescent="0.2">
       <c r="A7" s="17">
         <v>610</v>
       </c>
@@ -1556,24 +1588,25 @@
       <c r="K7" s="28">
         <v>6</v>
       </c>
-      <c r="L7" s="20"/>
-      <c r="M7" s="29">
+      <c r="L7" s="28"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="29">
         <v>18.03</v>
       </c>
-      <c r="N7" s="25">
+      <c r="O7" s="25">
         <v>13.522500000000001</v>
       </c>
-      <c r="O7" s="26">
+      <c r="P7" s="26">
         <v>12</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>51</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="17">
         <v>590</v>
       </c>
@@ -1608,23 +1641,24 @@
         <v>6</v>
       </c>
       <c r="L8" s="20"/>
-      <c r="M8" s="24">
+      <c r="M8" s="20"/>
+      <c r="N8" s="24">
         <v>16.260000000000002</v>
       </c>
-      <c r="N8" s="25">
+      <c r="O8" s="25">
         <v>12.195</v>
       </c>
-      <c r="O8" s="26">
+      <c r="P8" s="26">
         <v>12</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>54</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="17">
         <v>590</v>
       </c>
@@ -1659,23 +1693,24 @@
         <v>6</v>
       </c>
       <c r="L9" s="20"/>
-      <c r="M9" s="24">
+      <c r="M9" s="20"/>
+      <c r="N9" s="24">
         <v>16.260000000000002</v>
       </c>
-      <c r="N9" s="25">
+      <c r="O9" s="25">
         <v>20</v>
       </c>
-      <c r="O9" s="26">
+      <c r="P9" s="26">
         <v>12</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>54</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="29" x14ac:dyDescent="0.2">
       <c r="A10" s="17">
         <v>470</v>
       </c>
@@ -1709,23 +1744,24 @@
       <c r="K10" s="20">
         <v>10</v>
       </c>
-      <c r="L10" s="20">
+      <c r="L10" s="20"/>
+      <c r="M10" s="20">
         <v>5</v>
       </c>
-      <c r="M10" s="24">
+      <c r="N10" s="24">
         <v>16.420000000000002</v>
       </c>
-      <c r="N10" s="25">
+      <c r="O10" s="25">
         <v>10</v>
       </c>
-      <c r="O10" s="26">
+      <c r="P10" s="26">
         <v>12</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="29" x14ac:dyDescent="0.2">
       <c r="A11" s="17">
         <v>530</v>
       </c>
@@ -1757,21 +1793,24 @@
       <c r="K11" s="20">
         <v>6</v>
       </c>
-      <c r="L11" s="20"/>
-      <c r="M11" s="24">
+      <c r="L11" s="20">
+        <v>4</v>
+      </c>
+      <c r="M11" s="20"/>
+      <c r="N11" s="24">
         <v>13.72</v>
       </c>
-      <c r="N11" s="25">
+      <c r="O11" s="25">
         <v>10.29</v>
       </c>
-      <c r="O11" s="26">
+      <c r="P11" s="26">
         <v>12</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="17"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
@@ -1784,11 +1823,12 @@
       <c r="J12" s="23"/>
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="26"/>
-    </row>
-    <row r="13" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+      <c r="M12" s="20"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="26"/>
+    </row>
+    <row r="13" spans="1:18" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="17"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
@@ -1801,11 +1841,12 @@
       <c r="J13" s="23"/>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="26"/>
-    </row>
-    <row r="14" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+      <c r="M13" s="20"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="26"/>
+    </row>
+    <row r="14" spans="1:18" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -1818,11 +1859,12 @@
       <c r="J14" s="23"/>
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="26"/>
-    </row>
-    <row r="15" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+      <c r="M14" s="20"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="26"/>
+    </row>
+    <row r="15" spans="1:18" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
@@ -1835,11 +1877,12 @@
       <c r="J15" s="23"/>
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="26"/>
-    </row>
-    <row r="16" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+      <c r="M15" s="20"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="26"/>
+    </row>
+    <row r="16" spans="1:18" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
@@ -1852,11 +1895,12 @@
       <c r="J16" s="23"/>
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="26"/>
-    </row>
-    <row r="17" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M16" s="20"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="26"/>
+    </row>
+    <row r="17" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
       <c r="C17" s="19"/>
@@ -1869,11 +1913,12 @@
       <c r="J17" s="23"/>
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="26"/>
-    </row>
-    <row r="18" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M17" s="20"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="26"/>
+    </row>
+    <row r="18" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
       <c r="C18" s="19"/>
@@ -1886,11 +1931,12 @@
       <c r="J18" s="23"/>
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="26"/>
-    </row>
-    <row r="19" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M18" s="20"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="26"/>
+    </row>
+    <row r="19" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
       <c r="B19" s="18"/>
       <c r="C19" s="19"/>
@@ -1903,11 +1949,12 @@
       <c r="J19" s="23"/>
       <c r="K19" s="20"/>
       <c r="L19" s="20"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="25"/>
-      <c r="O19" s="26"/>
-    </row>
-    <row r="20" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M19" s="20"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="26"/>
+    </row>
+    <row r="20" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
       <c r="B20" s="18"/>
       <c r="C20" s="19"/>
@@ -1920,11 +1967,12 @@
       <c r="J20" s="23"/>
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="26"/>
-    </row>
-    <row r="21" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M20" s="20"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="26"/>
+    </row>
+    <row r="21" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19"/>
@@ -1937,11 +1985,12 @@
       <c r="J21" s="23"/>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="26"/>
-    </row>
-    <row r="22" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M21" s="20"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="26"/>
+    </row>
+    <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19"/>
@@ -1954,11 +2003,12 @@
       <c r="J22" s="23"/>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="26"/>
-    </row>
-    <row r="23" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M22" s="20"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="26"/>
+    </row>
+    <row r="23" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19"/>
@@ -1971,11 +2021,12 @@
       <c r="J23" s="23"/>
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="26"/>
-    </row>
-    <row r="24" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M23" s="20"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="25"/>
+      <c r="P23" s="26"/>
+    </row>
+    <row r="24" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="18"/>
       <c r="C24" s="19"/>
@@ -1988,11 +2039,12 @@
       <c r="J24" s="23"/>
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="26"/>
-    </row>
-    <row r="25" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M24" s="20"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="26"/>
+    </row>
+    <row r="25" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="18"/>
       <c r="C25" s="19"/>
@@ -2005,11 +2057,12 @@
       <c r="J25" s="23"/>
       <c r="K25" s="20"/>
       <c r="L25" s="20"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="26"/>
-    </row>
-    <row r="26" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M25" s="20"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="26"/>
+    </row>
+    <row r="26" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19"/>
@@ -2022,11 +2075,12 @@
       <c r="J26" s="23"/>
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="26"/>
-    </row>
-    <row r="27" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M26" s="20"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="26"/>
+    </row>
+    <row r="27" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="18"/>
       <c r="C27" s="19"/>
@@ -2039,11 +2093,12 @@
       <c r="J27" s="23"/>
       <c r="K27" s="20"/>
       <c r="L27" s="20"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="26"/>
-    </row>
-    <row r="28" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M27" s="20"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="26"/>
+    </row>
+    <row r="28" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
@@ -2056,11 +2111,12 @@
       <c r="J28" s="23"/>
       <c r="K28" s="20"/>
       <c r="L28" s="20"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="26"/>
-    </row>
-    <row r="29" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M28" s="20"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="26"/>
+    </row>
+    <row r="29" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="18"/>
       <c r="C29" s="19"/>
@@ -2073,11 +2129,12 @@
       <c r="J29" s="23"/>
       <c r="K29" s="20"/>
       <c r="L29" s="20"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="25"/>
-      <c r="O29" s="26"/>
-    </row>
-    <row r="30" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M29" s="20"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="25"/>
+      <c r="P29" s="26"/>
+    </row>
+    <row r="30" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
@@ -2090,11 +2147,12 @@
       <c r="J30" s="23"/>
       <c r="K30" s="20"/>
       <c r="L30" s="20"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="25"/>
-      <c r="O30" s="26"/>
-    </row>
-    <row r="31" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M30" s="20"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="25"/>
+      <c r="P30" s="26"/>
+    </row>
+    <row r="31" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="18"/>
       <c r="C31" s="19"/>
@@ -2107,11 +2165,12 @@
       <c r="J31" s="23"/>
       <c r="K31" s="20"/>
       <c r="L31" s="20"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="26"/>
-    </row>
-    <row r="32" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M31" s="20"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="25"/>
+      <c r="P31" s="26"/>
+    </row>
+    <row r="32" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="18"/>
       <c r="C32" s="19"/>
@@ -2124,11 +2183,12 @@
       <c r="J32" s="23"/>
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="25"/>
-      <c r="O32" s="26"/>
-    </row>
-    <row r="33" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M32" s="20"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="25"/>
+      <c r="P32" s="26"/>
+    </row>
+    <row r="33" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="18"/>
       <c r="C33" s="19"/>
@@ -2141,11 +2201,12 @@
       <c r="J33" s="23"/>
       <c r="K33" s="20"/>
       <c r="L33" s="20"/>
-      <c r="M33" s="24"/>
-      <c r="N33" s="25"/>
-      <c r="O33" s="26"/>
-    </row>
-    <row r="34" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M33" s="20"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="25"/>
+      <c r="P33" s="26"/>
+    </row>
+    <row r="34" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
@@ -2158,11 +2219,12 @@
       <c r="J34" s="23"/>
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
-      <c r="M34" s="24"/>
-      <c r="N34" s="25"/>
-      <c r="O34" s="26"/>
-    </row>
-    <row r="35" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M34" s="20"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="26"/>
+    </row>
+    <row r="35" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="18"/>
       <c r="C35" s="19"/>
@@ -2175,11 +2237,12 @@
       <c r="J35" s="23"/>
       <c r="K35" s="20"/>
       <c r="L35" s="20"/>
-      <c r="M35" s="24"/>
-      <c r="N35" s="25"/>
-      <c r="O35" s="26"/>
-    </row>
-    <row r="36" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M35" s="20"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="25"/>
+      <c r="P35" s="26"/>
+    </row>
+    <row r="36" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="18"/>
       <c r="C36" s="19"/>
@@ -2192,11 +2255,12 @@
       <c r="J36" s="23"/>
       <c r="K36" s="20"/>
       <c r="L36" s="20"/>
-      <c r="M36" s="24"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="26"/>
-    </row>
-    <row r="37" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M36" s="20"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="25"/>
+      <c r="P36" s="26"/>
+    </row>
+    <row r="37" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="18"/>
       <c r="C37" s="19"/>
@@ -2209,11 +2273,12 @@
       <c r="J37" s="23"/>
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
-      <c r="M37" s="24"/>
-      <c r="N37" s="25"/>
-      <c r="O37" s="26"/>
-    </row>
-    <row r="38" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M37" s="20"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="25"/>
+      <c r="P37" s="26"/>
+    </row>
+    <row r="38" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="18"/>
       <c r="C38" s="19"/>
@@ -2226,11 +2291,12 @@
       <c r="J38" s="23"/>
       <c r="K38" s="20"/>
       <c r="L38" s="20"/>
-      <c r="M38" s="24"/>
-      <c r="N38" s="25"/>
-      <c r="O38" s="26"/>
-    </row>
-    <row r="39" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M38" s="20"/>
+      <c r="N38" s="24"/>
+      <c r="O38" s="25"/>
+      <c r="P38" s="26"/>
+    </row>
+    <row r="39" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="18"/>
       <c r="C39" s="19"/>
@@ -2243,11 +2309,12 @@
       <c r="J39" s="23"/>
       <c r="K39" s="20"/>
       <c r="L39" s="20"/>
-      <c r="M39" s="24"/>
-      <c r="N39" s="25"/>
-      <c r="O39" s="26"/>
-    </row>
-    <row r="40" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M39" s="20"/>
+      <c r="N39" s="24"/>
+      <c r="O39" s="25"/>
+      <c r="P39" s="26"/>
+    </row>
+    <row r="40" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="18"/>
       <c r="C40" s="19"/>
@@ -2260,11 +2327,12 @@
       <c r="J40" s="23"/>
       <c r="K40" s="20"/>
       <c r="L40" s="20"/>
-      <c r="M40" s="24"/>
-      <c r="N40" s="25"/>
-      <c r="O40" s="26"/>
-    </row>
-    <row r="41" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M40" s="20"/>
+      <c r="N40" s="24"/>
+      <c r="O40" s="25"/>
+      <c r="P40" s="26"/>
+    </row>
+    <row r="41" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="18"/>
       <c r="C41" s="19"/>
@@ -2277,11 +2345,12 @@
       <c r="J41" s="23"/>
       <c r="K41" s="20"/>
       <c r="L41" s="20"/>
-      <c r="M41" s="24"/>
-      <c r="N41" s="25"/>
-      <c r="O41" s="26"/>
-    </row>
-    <row r="42" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M41" s="20"/>
+      <c r="N41" s="24"/>
+      <c r="O41" s="25"/>
+      <c r="P41" s="26"/>
+    </row>
+    <row r="42" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="18"/>
       <c r="C42" s="19"/>
@@ -2294,11 +2363,12 @@
       <c r="J42" s="23"/>
       <c r="K42" s="20"/>
       <c r="L42" s="20"/>
-      <c r="M42" s="24"/>
-      <c r="N42" s="25"/>
-      <c r="O42" s="26"/>
-    </row>
-    <row r="43" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M42" s="20"/>
+      <c r="N42" s="24"/>
+      <c r="O42" s="25"/>
+      <c r="P42" s="26"/>
+    </row>
+    <row r="43" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="18"/>
       <c r="C43" s="19"/>
@@ -2311,11 +2381,12 @@
       <c r="J43" s="23"/>
       <c r="K43" s="17"/>
       <c r="L43" s="17"/>
-      <c r="M43" s="24"/>
-      <c r="N43" s="25"/>
-      <c r="O43" s="26"/>
-    </row>
-    <row r="44" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M43" s="17"/>
+      <c r="N43" s="24"/>
+      <c r="O43" s="25"/>
+      <c r="P43" s="26"/>
+    </row>
+    <row r="44" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="32"/>
       <c r="C44" s="33"/>
@@ -2328,11 +2399,12 @@
       <c r="J44" s="23"/>
       <c r="K44" s="17"/>
       <c r="L44" s="17"/>
-      <c r="M44" s="24"/>
-      <c r="N44" s="25"/>
-      <c r="O44" s="26"/>
-    </row>
-    <row r="45" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M44" s="17"/>
+      <c r="N44" s="24"/>
+      <c r="O44" s="25"/>
+      <c r="P44" s="26"/>
+    </row>
+    <row r="45" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="34"/>
       <c r="C45" s="35"/>
@@ -2345,11 +2417,12 @@
       <c r="J45" s="23"/>
       <c r="K45" s="17"/>
       <c r="L45" s="17"/>
-      <c r="M45" s="36"/>
-      <c r="N45" s="25"/>
-      <c r="O45" s="26"/>
-    </row>
-    <row r="46" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M45" s="17"/>
+      <c r="N45" s="36"/>
+      <c r="O45" s="25"/>
+      <c r="P45" s="26"/>
+    </row>
+    <row r="46" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="34"/>
       <c r="C46" s="35"/>
@@ -2362,11 +2435,12 @@
       <c r="J46" s="23"/>
       <c r="K46" s="17"/>
       <c r="L46" s="17"/>
-      <c r="M46" s="36"/>
-      <c r="N46" s="25"/>
-      <c r="O46" s="26"/>
-    </row>
-    <row r="47" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M46" s="17"/>
+      <c r="N46" s="36"/>
+      <c r="O46" s="25"/>
+      <c r="P46" s="26"/>
+    </row>
+    <row r="47" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
       <c r="B47" s="34"/>
       <c r="C47" s="35"/>
@@ -2379,11 +2453,12 @@
       <c r="J47" s="23"/>
       <c r="K47" s="17"/>
       <c r="L47" s="17"/>
-      <c r="M47" s="36"/>
-      <c r="N47" s="25"/>
-      <c r="O47" s="26"/>
-    </row>
-    <row r="48" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M47" s="17"/>
+      <c r="N47" s="36"/>
+      <c r="O47" s="25"/>
+      <c r="P47" s="26"/>
+    </row>
+    <row r="48" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>
       <c r="B48" s="34"/>
       <c r="C48" s="35"/>
@@ -2396,11 +2471,12 @@
       <c r="J48" s="23"/>
       <c r="K48" s="17"/>
       <c r="L48" s="17"/>
-      <c r="M48" s="36"/>
-      <c r="N48" s="25"/>
-      <c r="O48" s="26"/>
-    </row>
-    <row r="49" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M48" s="17"/>
+      <c r="N48" s="36"/>
+      <c r="O48" s="25"/>
+      <c r="P48" s="26"/>
+    </row>
+    <row r="49" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
       <c r="B49" s="34"/>
       <c r="C49" s="35"/>
@@ -2413,11 +2489,12 @@
       <c r="J49" s="23"/>
       <c r="K49" s="17"/>
       <c r="L49" s="17"/>
-      <c r="M49" s="36"/>
-      <c r="N49" s="25"/>
-      <c r="O49" s="26"/>
-    </row>
-    <row r="50" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M49" s="17"/>
+      <c r="N49" s="36"/>
+      <c r="O49" s="25"/>
+      <c r="P49" s="26"/>
+    </row>
+    <row r="50" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>
       <c r="B50" s="34"/>
       <c r="C50" s="35"/>
@@ -2430,11 +2507,12 @@
       <c r="J50" s="23"/>
       <c r="K50" s="17"/>
       <c r="L50" s="17"/>
-      <c r="M50" s="36"/>
-      <c r="N50" s="25"/>
-      <c r="O50" s="26"/>
-    </row>
-    <row r="51" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M50" s="17"/>
+      <c r="N50" s="36"/>
+      <c r="O50" s="25"/>
+      <c r="P50" s="26"/>
+    </row>
+    <row r="51" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="17"/>
       <c r="B51" s="34"/>
       <c r="C51" s="35"/>
@@ -2447,11 +2525,12 @@
       <c r="J51" s="23"/>
       <c r="K51" s="17"/>
       <c r="L51" s="17"/>
-      <c r="M51" s="36"/>
-      <c r="N51" s="25"/>
-      <c r="O51" s="26"/>
-    </row>
-    <row r="52" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M51" s="17"/>
+      <c r="N51" s="36"/>
+      <c r="O51" s="25"/>
+      <c r="P51" s="26"/>
+    </row>
+    <row r="52" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="17"/>
       <c r="B52" s="34"/>
       <c r="C52" s="35"/>
@@ -2464,11 +2543,12 @@
       <c r="J52" s="23"/>
       <c r="K52" s="17"/>
       <c r="L52" s="17"/>
-      <c r="M52" s="36"/>
-      <c r="N52" s="25"/>
-      <c r="O52" s="26"/>
-    </row>
-    <row r="53" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M52" s="17"/>
+      <c r="N52" s="36"/>
+      <c r="O52" s="25"/>
+      <c r="P52" s="26"/>
+    </row>
+    <row r="53" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="17"/>
       <c r="B53" s="34"/>
       <c r="C53" s="35"/>
@@ -2481,11 +2561,12 @@
       <c r="J53" s="23"/>
       <c r="K53" s="17"/>
       <c r="L53" s="17"/>
-      <c r="M53" s="36"/>
-      <c r="N53" s="25"/>
-      <c r="O53" s="26"/>
-    </row>
-    <row r="54" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M53" s="17"/>
+      <c r="N53" s="36"/>
+      <c r="O53" s="25"/>
+      <c r="P53" s="26"/>
+    </row>
+    <row r="54" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="17"/>
       <c r="B54" s="34"/>
       <c r="C54" s="35"/>
@@ -2498,11 +2579,12 @@
       <c r="J54" s="23"/>
       <c r="K54" s="17"/>
       <c r="L54" s="17"/>
-      <c r="M54" s="36"/>
-      <c r="N54" s="25"/>
-      <c r="O54" s="26"/>
-    </row>
-    <row r="55" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M54" s="17"/>
+      <c r="N54" s="36"/>
+      <c r="O54" s="25"/>
+      <c r="P54" s="26"/>
+    </row>
+    <row r="55" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="17"/>
       <c r="B55" s="34"/>
       <c r="C55" s="35"/>
@@ -2515,11 +2597,12 @@
       <c r="J55" s="23"/>
       <c r="K55" s="17"/>
       <c r="L55" s="17"/>
-      <c r="M55" s="36"/>
-      <c r="N55" s="25"/>
-      <c r="O55" s="26"/>
-    </row>
-    <row r="56" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M55" s="17"/>
+      <c r="N55" s="36"/>
+      <c r="O55" s="25"/>
+      <c r="P55" s="26"/>
+    </row>
+    <row r="56" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="17"/>
       <c r="B56" s="34"/>
       <c r="C56" s="35"/>
@@ -2532,11 +2615,12 @@
       <c r="J56" s="23"/>
       <c r="K56" s="17"/>
       <c r="L56" s="17"/>
-      <c r="M56" s="36"/>
-      <c r="N56" s="25"/>
-      <c r="O56" s="26"/>
-    </row>
-    <row r="57" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M56" s="17"/>
+      <c r="N56" s="36"/>
+      <c r="O56" s="25"/>
+      <c r="P56" s="26"/>
+    </row>
+    <row r="57" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="17"/>
       <c r="B57" s="34"/>
       <c r="C57" s="35"/>
@@ -2549,11 +2633,12 @@
       <c r="J57" s="23"/>
       <c r="K57" s="17"/>
       <c r="L57" s="17"/>
-      <c r="M57" s="36"/>
-      <c r="N57" s="25"/>
-      <c r="O57" s="26"/>
-    </row>
-    <row r="58" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M57" s="17"/>
+      <c r="N57" s="36"/>
+      <c r="O57" s="25"/>
+      <c r="P57" s="26"/>
+    </row>
+    <row r="58" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="17"/>
       <c r="B58" s="34"/>
       <c r="C58" s="35"/>
@@ -2566,11 +2651,12 @@
       <c r="J58" s="23"/>
       <c r="K58" s="17"/>
       <c r="L58" s="17"/>
-      <c r="M58" s="36"/>
-      <c r="N58" s="25"/>
-      <c r="O58" s="26"/>
-    </row>
-    <row r="59" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M58" s="17"/>
+      <c r="N58" s="36"/>
+      <c r="O58" s="25"/>
+      <c r="P58" s="26"/>
+    </row>
+    <row r="59" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="17"/>
       <c r="B59" s="34"/>
       <c r="C59" s="35"/>
@@ -2583,11 +2669,12 @@
       <c r="J59" s="23"/>
       <c r="K59" s="17"/>
       <c r="L59" s="17"/>
-      <c r="M59" s="36"/>
-      <c r="N59" s="25"/>
-      <c r="O59" s="26"/>
-    </row>
-    <row r="60" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M59" s="17"/>
+      <c r="N59" s="36"/>
+      <c r="O59" s="25"/>
+      <c r="P59" s="26"/>
+    </row>
+    <row r="60" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="17"/>
       <c r="B60" s="34"/>
       <c r="C60" s="35"/>
@@ -2600,11 +2687,12 @@
       <c r="J60" s="23"/>
       <c r="K60" s="17"/>
       <c r="L60" s="17"/>
-      <c r="M60" s="36"/>
-      <c r="N60" s="25"/>
-      <c r="O60" s="26"/>
-    </row>
-    <row r="61" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M60" s="17"/>
+      <c r="N60" s="36"/>
+      <c r="O60" s="25"/>
+      <c r="P60" s="26"/>
+    </row>
+    <row r="61" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="17"/>
       <c r="B61" s="34"/>
       <c r="C61" s="35"/>
@@ -2617,11 +2705,12 @@
       <c r="J61" s="23"/>
       <c r="K61" s="17"/>
       <c r="L61" s="17"/>
-      <c r="M61" s="36"/>
-      <c r="N61" s="25"/>
-      <c r="O61" s="26"/>
-    </row>
-    <row r="62" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M61" s="17"/>
+      <c r="N61" s="36"/>
+      <c r="O61" s="25"/>
+      <c r="P61" s="26"/>
+    </row>
+    <row r="62" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="17"/>
       <c r="B62" s="34"/>
       <c r="C62" s="35"/>
@@ -2634,11 +2723,12 @@
       <c r="J62" s="23"/>
       <c r="K62" s="17"/>
       <c r="L62" s="17"/>
-      <c r="M62" s="36"/>
-      <c r="N62" s="25"/>
-      <c r="O62" s="26"/>
-    </row>
-    <row r="63" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M62" s="17"/>
+      <c r="N62" s="36"/>
+      <c r="O62" s="25"/>
+      <c r="P62" s="26"/>
+    </row>
+    <row r="63" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="17"/>
       <c r="B63" s="34"/>
       <c r="C63" s="35"/>
@@ -2651,11 +2741,12 @@
       <c r="J63" s="23"/>
       <c r="K63" s="17"/>
       <c r="L63" s="17"/>
-      <c r="M63" s="36"/>
-      <c r="N63" s="25"/>
-      <c r="O63" s="26"/>
-    </row>
-    <row r="64" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M63" s="17"/>
+      <c r="N63" s="36"/>
+      <c r="O63" s="25"/>
+      <c r="P63" s="26"/>
+    </row>
+    <row r="64" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" s="17"/>
       <c r="B64" s="34"/>
       <c r="C64" s="35"/>
@@ -2668,11 +2759,12 @@
       <c r="J64" s="23"/>
       <c r="K64" s="17"/>
       <c r="L64" s="17"/>
-      <c r="M64" s="36"/>
-      <c r="N64" s="25"/>
-      <c r="O64" s="26"/>
-    </row>
-    <row r="65" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M64" s="17"/>
+      <c r="N64" s="36"/>
+      <c r="O64" s="25"/>
+      <c r="P64" s="26"/>
+    </row>
+    <row r="65" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="17"/>
       <c r="B65" s="34"/>
       <c r="C65" s="35"/>
@@ -2685,11 +2777,12 @@
       <c r="J65" s="23"/>
       <c r="K65" s="17"/>
       <c r="L65" s="17"/>
-      <c r="M65" s="36"/>
-      <c r="N65" s="25"/>
-      <c r="O65" s="26"/>
-    </row>
-    <row r="66" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M65" s="17"/>
+      <c r="N65" s="36"/>
+      <c r="O65" s="25"/>
+      <c r="P65" s="26"/>
+    </row>
+    <row r="66" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" s="17"/>
       <c r="B66" s="34"/>
       <c r="C66" s="35"/>
@@ -2702,11 +2795,12 @@
       <c r="J66" s="23"/>
       <c r="K66" s="17"/>
       <c r="L66" s="17"/>
-      <c r="M66" s="36"/>
-      <c r="N66" s="25"/>
-      <c r="O66" s="26"/>
-    </row>
-    <row r="67" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M66" s="17"/>
+      <c r="N66" s="36"/>
+      <c r="O66" s="25"/>
+      <c r="P66" s="26"/>
+    </row>
+    <row r="67" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="17"/>
       <c r="B67" s="34"/>
       <c r="C67" s="35"/>
@@ -2719,11 +2813,12 @@
       <c r="J67" s="23"/>
       <c r="K67" s="17"/>
       <c r="L67" s="17"/>
-      <c r="M67" s="36"/>
-      <c r="N67" s="25"/>
-      <c r="O67" s="26"/>
-    </row>
-    <row r="68" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M67" s="17"/>
+      <c r="N67" s="36"/>
+      <c r="O67" s="25"/>
+      <c r="P67" s="26"/>
+    </row>
+    <row r="68" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="17"/>
       <c r="B68" s="34"/>
       <c r="C68" s="35"/>
@@ -2736,11 +2831,12 @@
       <c r="J68" s="23"/>
       <c r="K68" s="17"/>
       <c r="L68" s="17"/>
-      <c r="M68" s="36"/>
-      <c r="N68" s="25"/>
-      <c r="O68" s="26"/>
-    </row>
-    <row r="69" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M68" s="17"/>
+      <c r="N68" s="36"/>
+      <c r="O68" s="25"/>
+      <c r="P68" s="26"/>
+    </row>
+    <row r="69" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="17"/>
       <c r="B69" s="34"/>
       <c r="C69" s="35"/>
@@ -2753,11 +2849,12 @@
       <c r="J69" s="23"/>
       <c r="K69" s="17"/>
       <c r="L69" s="17"/>
-      <c r="M69" s="36"/>
-      <c r="N69" s="25"/>
-      <c r="O69" s="26"/>
-    </row>
-    <row r="70" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M69" s="17"/>
+      <c r="N69" s="36"/>
+      <c r="O69" s="25"/>
+      <c r="P69" s="26"/>
+    </row>
+    <row r="70" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="17"/>
       <c r="B70" s="34"/>
       <c r="C70" s="35"/>
@@ -2770,11 +2867,12 @@
       <c r="J70" s="23"/>
       <c r="K70" s="17"/>
       <c r="L70" s="17"/>
-      <c r="M70" s="36"/>
-      <c r="N70" s="25"/>
-      <c r="O70" s="26"/>
-    </row>
-    <row r="71" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M70" s="17"/>
+      <c r="N70" s="36"/>
+      <c r="O70" s="25"/>
+      <c r="P70" s="26"/>
+    </row>
+    <row r="71" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="17"/>
       <c r="B71" s="34"/>
       <c r="C71" s="35"/>
@@ -2787,11 +2885,12 @@
       <c r="J71" s="23"/>
       <c r="K71" s="17"/>
       <c r="L71" s="17"/>
-      <c r="M71" s="36"/>
-      <c r="N71" s="25"/>
-      <c r="O71" s="26"/>
-    </row>
-    <row r="72" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M71" s="17"/>
+      <c r="N71" s="36"/>
+      <c r="O71" s="25"/>
+      <c r="P71" s="26"/>
+    </row>
+    <row r="72" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="17"/>
       <c r="B72" s="34"/>
       <c r="C72" s="35"/>
@@ -2804,11 +2903,12 @@
       <c r="J72" s="23"/>
       <c r="K72" s="17"/>
       <c r="L72" s="17"/>
-      <c r="M72" s="36"/>
-      <c r="N72" s="25"/>
-      <c r="O72" s="26"/>
-    </row>
-    <row r="73" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M72" s="17"/>
+      <c r="N72" s="36"/>
+      <c r="O72" s="25"/>
+      <c r="P72" s="26"/>
+    </row>
+    <row r="73" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="17"/>
       <c r="B73" s="34"/>
       <c r="C73" s="35"/>
@@ -2821,11 +2921,12 @@
       <c r="J73" s="23"/>
       <c r="K73" s="17"/>
       <c r="L73" s="17"/>
-      <c r="M73" s="36"/>
-      <c r="N73" s="25"/>
-      <c r="O73" s="26"/>
-    </row>
-    <row r="74" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M73" s="17"/>
+      <c r="N73" s="36"/>
+      <c r="O73" s="25"/>
+      <c r="P73" s="26"/>
+    </row>
+    <row r="74" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="17"/>
       <c r="B74" s="34"/>
       <c r="C74" s="35"/>
@@ -2838,11 +2939,12 @@
       <c r="J74" s="23"/>
       <c r="K74" s="17"/>
       <c r="L74" s="17"/>
-      <c r="M74" s="36"/>
-      <c r="N74" s="25"/>
-      <c r="O74" s="26"/>
-    </row>
-    <row r="75" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M74" s="17"/>
+      <c r="N74" s="36"/>
+      <c r="O74" s="25"/>
+      <c r="P74" s="26"/>
+    </row>
+    <row r="75" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="17"/>
       <c r="B75" s="34"/>
       <c r="C75" s="35"/>
@@ -2855,11 +2957,12 @@
       <c r="J75" s="23"/>
       <c r="K75" s="17"/>
       <c r="L75" s="17"/>
-      <c r="M75" s="36"/>
-      <c r="N75" s="25"/>
-      <c r="O75" s="26"/>
-    </row>
-    <row r="76" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M75" s="17"/>
+      <c r="N75" s="36"/>
+      <c r="O75" s="25"/>
+      <c r="P75" s="26"/>
+    </row>
+    <row r="76" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" s="17"/>
       <c r="B76" s="34"/>
       <c r="C76" s="35"/>
@@ -2872,11 +2975,12 @@
       <c r="J76" s="23"/>
       <c r="K76" s="17"/>
       <c r="L76" s="17"/>
-      <c r="M76" s="36"/>
-      <c r="N76" s="25"/>
-      <c r="O76" s="26"/>
-    </row>
-    <row r="77" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M76" s="17"/>
+      <c r="N76" s="36"/>
+      <c r="O76" s="25"/>
+      <c r="P76" s="26"/>
+    </row>
+    <row r="77" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" s="17"/>
       <c r="B77" s="34"/>
       <c r="C77" s="35"/>
@@ -2889,11 +2993,12 @@
       <c r="J77" s="23"/>
       <c r="K77" s="17"/>
       <c r="L77" s="17"/>
-      <c r="M77" s="36"/>
-      <c r="N77" s="25"/>
-      <c r="O77" s="26"/>
-    </row>
-    <row r="78" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M77" s="17"/>
+      <c r="N77" s="36"/>
+      <c r="O77" s="25"/>
+      <c r="P77" s="26"/>
+    </row>
+    <row r="78" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" s="17"/>
       <c r="B78" s="34"/>
       <c r="C78" s="35"/>
@@ -2906,11 +3011,12 @@
       <c r="J78" s="23"/>
       <c r="K78" s="17"/>
       <c r="L78" s="17"/>
-      <c r="M78" s="36"/>
-      <c r="N78" s="25"/>
-      <c r="O78" s="26"/>
-    </row>
-    <row r="79" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M78" s="17"/>
+      <c r="N78" s="36"/>
+      <c r="O78" s="25"/>
+      <c r="P78" s="26"/>
+    </row>
+    <row r="79" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" s="17"/>
       <c r="B79" s="34"/>
       <c r="C79" s="35"/>
@@ -2923,11 +3029,12 @@
       <c r="J79" s="23"/>
       <c r="K79" s="17"/>
       <c r="L79" s="17"/>
-      <c r="M79" s="36"/>
-      <c r="N79" s="25"/>
-      <c r="O79" s="26"/>
-    </row>
-    <row r="80" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M79" s="17"/>
+      <c r="N79" s="36"/>
+      <c r="O79" s="25"/>
+      <c r="P79" s="26"/>
+    </row>
+    <row r="80" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="17"/>
       <c r="B80" s="34"/>
       <c r="C80" s="35"/>
@@ -2940,11 +3047,12 @@
       <c r="J80" s="23"/>
       <c r="K80" s="17"/>
       <c r="L80" s="17"/>
-      <c r="M80" s="36"/>
-      <c r="N80" s="25"/>
-      <c r="O80" s="26"/>
-    </row>
-    <row r="81" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M80" s="17"/>
+      <c r="N80" s="36"/>
+      <c r="O80" s="25"/>
+      <c r="P80" s="26"/>
+    </row>
+    <row r="81" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" s="17"/>
       <c r="B81" s="34"/>
       <c r="C81" s="35"/>
@@ -2957,11 +3065,12 @@
       <c r="J81" s="23"/>
       <c r="K81" s="17"/>
       <c r="L81" s="17"/>
-      <c r="M81" s="36"/>
-      <c r="N81" s="25"/>
-      <c r="O81" s="26"/>
-    </row>
-    <row r="82" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M81" s="17"/>
+      <c r="N81" s="36"/>
+      <c r="O81" s="25"/>
+      <c r="P81" s="26"/>
+    </row>
+    <row r="82" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" s="17"/>
       <c r="B82" s="34"/>
       <c r="C82" s="35"/>
@@ -2974,11 +3083,12 @@
       <c r="J82" s="23"/>
       <c r="K82" s="17"/>
       <c r="L82" s="17"/>
-      <c r="M82" s="36"/>
-      <c r="N82" s="25"/>
-      <c r="O82" s="26"/>
-    </row>
-    <row r="83" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M82" s="17"/>
+      <c r="N82" s="36"/>
+      <c r="O82" s="25"/>
+      <c r="P82" s="26"/>
+    </row>
+    <row r="83" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" s="17"/>
       <c r="B83" s="34"/>
       <c r="C83" s="35"/>
@@ -2991,11 +3101,12 @@
       <c r="J83" s="23"/>
       <c r="K83" s="17"/>
       <c r="L83" s="17"/>
-      <c r="M83" s="36"/>
-      <c r="N83" s="25"/>
-      <c r="O83" s="26"/>
-    </row>
-    <row r="84" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M83" s="17"/>
+      <c r="N83" s="36"/>
+      <c r="O83" s="25"/>
+      <c r="P83" s="26"/>
+    </row>
+    <row r="84" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" s="17"/>
       <c r="B84" s="34"/>
       <c r="C84" s="35"/>
@@ -3008,11 +3119,12 @@
       <c r="J84" s="23"/>
       <c r="K84" s="17"/>
       <c r="L84" s="17"/>
-      <c r="M84" s="36"/>
-      <c r="N84" s="25"/>
-      <c r="O84" s="26"/>
-    </row>
-    <row r="85" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M84" s="17"/>
+      <c r="N84" s="36"/>
+      <c r="O84" s="25"/>
+      <c r="P84" s="26"/>
+    </row>
+    <row r="85" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" s="17"/>
       <c r="B85" s="34"/>
       <c r="C85" s="35"/>
@@ -3025,11 +3137,12 @@
       <c r="J85" s="23"/>
       <c r="K85" s="17"/>
       <c r="L85" s="17"/>
-      <c r="M85" s="36"/>
-      <c r="N85" s="25"/>
-      <c r="O85" s="26"/>
-    </row>
-    <row r="86" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M85" s="17"/>
+      <c r="N85" s="36"/>
+      <c r="O85" s="25"/>
+      <c r="P85" s="26"/>
+    </row>
+    <row r="86" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" s="17"/>
       <c r="B86" s="34"/>
       <c r="C86" s="35"/>
@@ -3042,11 +3155,12 @@
       <c r="J86" s="23"/>
       <c r="K86" s="17"/>
       <c r="L86" s="17"/>
-      <c r="M86" s="36"/>
-      <c r="N86" s="25"/>
-      <c r="O86" s="26"/>
-    </row>
-    <row r="87" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M86" s="17"/>
+      <c r="N86" s="36"/>
+      <c r="O86" s="25"/>
+      <c r="P86" s="26"/>
+    </row>
+    <row r="87" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" s="17"/>
       <c r="B87" s="34"/>
       <c r="C87" s="35"/>
@@ -3059,11 +3173,12 @@
       <c r="J87" s="23"/>
       <c r="K87" s="17"/>
       <c r="L87" s="17"/>
-      <c r="M87" s="36"/>
-      <c r="N87" s="25"/>
-      <c r="O87" s="26"/>
-    </row>
-    <row r="88" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M87" s="17"/>
+      <c r="N87" s="36"/>
+      <c r="O87" s="25"/>
+      <c r="P87" s="26"/>
+    </row>
+    <row r="88" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="17"/>
       <c r="B88" s="34"/>
       <c r="C88" s="35"/>
@@ -3076,11 +3191,12 @@
       <c r="J88" s="23"/>
       <c r="K88" s="17"/>
       <c r="L88" s="17"/>
-      <c r="M88" s="36"/>
-      <c r="N88" s="25"/>
-      <c r="O88" s="26"/>
-    </row>
-    <row r="89" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M88" s="17"/>
+      <c r="N88" s="36"/>
+      <c r="O88" s="25"/>
+      <c r="P88" s="26"/>
+    </row>
+    <row r="89" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A89" s="17"/>
       <c r="B89" s="34"/>
       <c r="C89" s="35"/>
@@ -3093,11 +3209,12 @@
       <c r="J89" s="23"/>
       <c r="K89" s="17"/>
       <c r="L89" s="17"/>
-      <c r="M89" s="36"/>
-      <c r="N89" s="25"/>
-      <c r="O89" s="26"/>
-    </row>
-    <row r="90" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M89" s="17"/>
+      <c r="N89" s="36"/>
+      <c r="O89" s="25"/>
+      <c r="P89" s="26"/>
+    </row>
+    <row r="90" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A90" s="17"/>
       <c r="B90" s="34"/>
       <c r="C90" s="35"/>
@@ -3110,11 +3227,12 @@
       <c r="J90" s="23"/>
       <c r="K90" s="17"/>
       <c r="L90" s="17"/>
-      <c r="M90" s="36"/>
-      <c r="N90" s="25"/>
-      <c r="O90" s="26"/>
-    </row>
-    <row r="91" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M90" s="17"/>
+      <c r="N90" s="36"/>
+      <c r="O90" s="25"/>
+      <c r="P90" s="26"/>
+    </row>
+    <row r="91" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" s="17"/>
       <c r="B91" s="34"/>
       <c r="C91" s="35"/>
@@ -3127,11 +3245,12 @@
       <c r="J91" s="23"/>
       <c r="K91" s="17"/>
       <c r="L91" s="17"/>
-      <c r="M91" s="36"/>
-      <c r="N91" s="25"/>
-      <c r="O91" s="26"/>
-    </row>
-    <row r="92" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M91" s="17"/>
+      <c r="N91" s="36"/>
+      <c r="O91" s="25"/>
+      <c r="P91" s="26"/>
+    </row>
+    <row r="92" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" s="17"/>
       <c r="B92" s="34"/>
       <c r="C92" s="35"/>
@@ -3144,11 +3263,12 @@
       <c r="J92" s="23"/>
       <c r="K92" s="17"/>
       <c r="L92" s="17"/>
-      <c r="M92" s="36"/>
-      <c r="N92" s="25"/>
-      <c r="O92" s="26"/>
-    </row>
-    <row r="93" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M92" s="17"/>
+      <c r="N92" s="36"/>
+      <c r="O92" s="25"/>
+      <c r="P92" s="26"/>
+    </row>
+    <row r="93" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" s="17"/>
       <c r="B93" s="34"/>
       <c r="C93" s="35"/>
@@ -3161,11 +3281,12 @@
       <c r="J93" s="23"/>
       <c r="K93" s="17"/>
       <c r="L93" s="17"/>
-      <c r="M93" s="36"/>
-      <c r="N93" s="25"/>
-      <c r="O93" s="26"/>
-    </row>
-    <row r="94" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M93" s="17"/>
+      <c r="N93" s="36"/>
+      <c r="O93" s="25"/>
+      <c r="P93" s="26"/>
+    </row>
+    <row r="94" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A94" s="17"/>
       <c r="B94" s="34"/>
       <c r="C94" s="35"/>
@@ -3178,11 +3299,12 @@
       <c r="J94" s="23"/>
       <c r="K94" s="17"/>
       <c r="L94" s="17"/>
-      <c r="M94" s="36"/>
-      <c r="N94" s="25"/>
-      <c r="O94" s="26"/>
-    </row>
-    <row r="95" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M94" s="17"/>
+      <c r="N94" s="36"/>
+      <c r="O94" s="25"/>
+      <c r="P94" s="26"/>
+    </row>
+    <row r="95" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A95" s="17"/>
       <c r="B95" s="34"/>
       <c r="C95" s="35"/>
@@ -3195,11 +3317,12 @@
       <c r="J95" s="23"/>
       <c r="K95" s="17"/>
       <c r="L95" s="17"/>
-      <c r="M95" s="36"/>
-      <c r="N95" s="25"/>
-      <c r="O95" s="26"/>
-    </row>
-    <row r="96" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M95" s="17"/>
+      <c r="N95" s="36"/>
+      <c r="O95" s="25"/>
+      <c r="P95" s="26"/>
+    </row>
+    <row r="96" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" s="17"/>
       <c r="B96" s="34"/>
       <c r="C96" s="35"/>
@@ -3212,11 +3335,12 @@
       <c r="J96" s="23"/>
       <c r="K96" s="17"/>
       <c r="L96" s="17"/>
-      <c r="M96" s="36"/>
-      <c r="N96" s="25"/>
-      <c r="O96" s="26"/>
-    </row>
-    <row r="97" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M96" s="17"/>
+      <c r="N96" s="36"/>
+      <c r="O96" s="25"/>
+      <c r="P96" s="26"/>
+    </row>
+    <row r="97" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A97" s="17"/>
       <c r="B97" s="34"/>
       <c r="C97" s="35"/>
@@ -3229,11 +3353,12 @@
       <c r="J97" s="23"/>
       <c r="K97" s="17"/>
       <c r="L97" s="17"/>
-      <c r="M97" s="36"/>
-      <c r="N97" s="25"/>
-      <c r="O97" s="26"/>
-    </row>
-    <row r="98" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M97" s="17"/>
+      <c r="N97" s="36"/>
+      <c r="O97" s="25"/>
+      <c r="P97" s="26"/>
+    </row>
+    <row r="98" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A98" s="17"/>
       <c r="B98" s="34"/>
       <c r="C98" s="35"/>
@@ -3246,11 +3371,12 @@
       <c r="J98" s="23"/>
       <c r="K98" s="17"/>
       <c r="L98" s="17"/>
-      <c r="M98" s="36"/>
-      <c r="N98" s="25"/>
-      <c r="O98" s="26"/>
-    </row>
-    <row r="99" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M98" s="17"/>
+      <c r="N98" s="36"/>
+      <c r="O98" s="25"/>
+      <c r="P98" s="26"/>
+    </row>
+    <row r="99" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A99" s="17"/>
       <c r="B99" s="34"/>
       <c r="C99" s="35"/>
@@ -3263,11 +3389,12 @@
       <c r="J99" s="23"/>
       <c r="K99" s="17"/>
       <c r="L99" s="17"/>
-      <c r="M99" s="36"/>
-      <c r="N99" s="25"/>
-      <c r="O99" s="26"/>
-    </row>
-    <row r="100" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M99" s="17"/>
+      <c r="N99" s="36"/>
+      <c r="O99" s="25"/>
+      <c r="P99" s="26"/>
+    </row>
+    <row r="100" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A100" s="17"/>
       <c r="B100" s="34"/>
       <c r="C100" s="35"/>
@@ -3280,11 +3407,12 @@
       <c r="J100" s="23"/>
       <c r="K100" s="17"/>
       <c r="L100" s="17"/>
-      <c r="M100" s="36"/>
-      <c r="N100" s="25"/>
-      <c r="O100" s="26"/>
-    </row>
-    <row r="101" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M100" s="17"/>
+      <c r="N100" s="36"/>
+      <c r="O100" s="25"/>
+      <c r="P100" s="26"/>
+    </row>
+    <row r="101" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A101" s="17"/>
       <c r="B101" s="34"/>
       <c r="C101" s="35"/>
@@ -3297,11 +3425,12 @@
       <c r="J101" s="23"/>
       <c r="K101" s="17"/>
       <c r="L101" s="17"/>
-      <c r="M101" s="36"/>
-      <c r="N101" s="25"/>
-      <c r="O101" s="26"/>
-    </row>
-    <row r="102" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M101" s="17"/>
+      <c r="N101" s="36"/>
+      <c r="O101" s="25"/>
+      <c r="P101" s="26"/>
+    </row>
+    <row r="102" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A102" s="17"/>
       <c r="B102" s="34"/>
       <c r="C102" s="35"/>
@@ -3314,11 +3443,12 @@
       <c r="J102" s="23"/>
       <c r="K102" s="17"/>
       <c r="L102" s="17"/>
-      <c r="M102" s="36"/>
-      <c r="N102" s="25"/>
-      <c r="O102" s="26"/>
-    </row>
-    <row r="103" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M102" s="17"/>
+      <c r="N102" s="36"/>
+      <c r="O102" s="25"/>
+      <c r="P102" s="26"/>
+    </row>
+    <row r="103" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A103" s="17"/>
       <c r="B103" s="34"/>
       <c r="C103" s="35"/>
@@ -3331,11 +3461,12 @@
       <c r="J103" s="23"/>
       <c r="K103" s="17"/>
       <c r="L103" s="17"/>
-      <c r="M103" s="36"/>
-      <c r="N103" s="25"/>
-      <c r="O103" s="26"/>
-    </row>
-    <row r="104" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M103" s="17"/>
+      <c r="N103" s="36"/>
+      <c r="O103" s="25"/>
+      <c r="P103" s="26"/>
+    </row>
+    <row r="104" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A104" s="17"/>
       <c r="B104" s="34"/>
       <c r="C104" s="35"/>
@@ -3348,11 +3479,12 @@
       <c r="J104" s="23"/>
       <c r="K104" s="17"/>
       <c r="L104" s="17"/>
-      <c r="M104" s="36"/>
-      <c r="N104" s="25"/>
-      <c r="O104" s="26"/>
-    </row>
-    <row r="105" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M104" s="17"/>
+      <c r="N104" s="36"/>
+      <c r="O104" s="25"/>
+      <c r="P104" s="26"/>
+    </row>
+    <row r="105" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A105" s="17"/>
       <c r="B105" s="34"/>
       <c r="C105" s="35"/>
@@ -3365,11 +3497,12 @@
       <c r="J105" s="23"/>
       <c r="K105" s="17"/>
       <c r="L105" s="17"/>
-      <c r="M105" s="36"/>
-      <c r="N105" s="25"/>
-      <c r="O105" s="26"/>
-    </row>
-    <row r="106" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M105" s="17"/>
+      <c r="N105" s="36"/>
+      <c r="O105" s="25"/>
+      <c r="P105" s="26"/>
+    </row>
+    <row r="106" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A106" s="17"/>
       <c r="B106" s="34"/>
       <c r="C106" s="35"/>
@@ -3382,11 +3515,12 @@
       <c r="J106" s="23"/>
       <c r="K106" s="17"/>
       <c r="L106" s="17"/>
-      <c r="M106" s="36"/>
-      <c r="N106" s="25"/>
-      <c r="O106" s="26"/>
-    </row>
-    <row r="107" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M106" s="17"/>
+      <c r="N106" s="36"/>
+      <c r="O106" s="25"/>
+      <c r="P106" s="26"/>
+    </row>
+    <row r="107" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A107" s="17"/>
       <c r="B107" s="34"/>
       <c r="C107" s="35"/>
@@ -3399,11 +3533,12 @@
       <c r="J107" s="23"/>
       <c r="K107" s="17"/>
       <c r="L107" s="17"/>
-      <c r="M107" s="36"/>
-      <c r="N107" s="25"/>
-      <c r="O107" s="26"/>
-    </row>
-    <row r="108" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M107" s="17"/>
+      <c r="N107" s="36"/>
+      <c r="O107" s="25"/>
+      <c r="P107" s="26"/>
+    </row>
+    <row r="108" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A108" s="17"/>
       <c r="B108" s="34"/>
       <c r="C108" s="35"/>
@@ -3416,11 +3551,12 @@
       <c r="J108" s="23"/>
       <c r="K108" s="17"/>
       <c r="L108" s="17"/>
-      <c r="M108" s="36"/>
-      <c r="N108" s="25"/>
-      <c r="O108" s="26"/>
-    </row>
-    <row r="109" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M108" s="17"/>
+      <c r="N108" s="36"/>
+      <c r="O108" s="25"/>
+      <c r="P108" s="26"/>
+    </row>
+    <row r="109" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A109" s="17"/>
       <c r="B109" s="34"/>
       <c r="C109" s="35"/>
@@ -3433,11 +3569,12 @@
       <c r="J109" s="23"/>
       <c r="K109" s="17"/>
       <c r="L109" s="17"/>
-      <c r="M109" s="36"/>
-      <c r="N109" s="25"/>
-      <c r="O109" s="26"/>
-    </row>
-    <row r="110" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M109" s="17"/>
+      <c r="N109" s="36"/>
+      <c r="O109" s="25"/>
+      <c r="P109" s="26"/>
+    </row>
+    <row r="110" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A110" s="17"/>
       <c r="B110" s="34"/>
       <c r="C110" s="35"/>
@@ -3450,11 +3587,12 @@
       <c r="J110" s="23"/>
       <c r="K110" s="17"/>
       <c r="L110" s="17"/>
-      <c r="M110" s="36"/>
-      <c r="N110" s="25"/>
-      <c r="O110" s="26"/>
-    </row>
-    <row r="111" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M110" s="17"/>
+      <c r="N110" s="36"/>
+      <c r="O110" s="25"/>
+      <c r="P110" s="26"/>
+    </row>
+    <row r="111" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A111" s="17"/>
       <c r="B111" s="34"/>
       <c r="C111" s="35"/>
@@ -3467,11 +3605,12 @@
       <c r="J111" s="23"/>
       <c r="K111" s="17"/>
       <c r="L111" s="17"/>
-      <c r="M111" s="36"/>
-      <c r="N111" s="25"/>
-      <c r="O111" s="26"/>
-    </row>
-    <row r="112" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M111" s="17"/>
+      <c r="N111" s="36"/>
+      <c r="O111" s="25"/>
+      <c r="P111" s="26"/>
+    </row>
+    <row r="112" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A112" s="17"/>
       <c r="B112" s="34"/>
       <c r="C112" s="35"/>
@@ -3484,11 +3623,12 @@
       <c r="J112" s="23"/>
       <c r="K112" s="17"/>
       <c r="L112" s="17"/>
-      <c r="M112" s="36"/>
-      <c r="N112" s="25"/>
-      <c r="O112" s="26"/>
-    </row>
-    <row r="113" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M112" s="17"/>
+      <c r="N112" s="36"/>
+      <c r="O112" s="25"/>
+      <c r="P112" s="26"/>
+    </row>
+    <row r="113" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A113" s="17"/>
       <c r="B113" s="34"/>
       <c r="C113" s="35"/>
@@ -3501,11 +3641,12 @@
       <c r="J113" s="23"/>
       <c r="K113" s="17"/>
       <c r="L113" s="17"/>
-      <c r="M113" s="36"/>
-      <c r="N113" s="25"/>
-      <c r="O113" s="26"/>
-    </row>
-    <row r="114" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M113" s="17"/>
+      <c r="N113" s="36"/>
+      <c r="O113" s="25"/>
+      <c r="P113" s="26"/>
+    </row>
+    <row r="114" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A114" s="17"/>
       <c r="B114" s="34"/>
       <c r="C114" s="35"/>
@@ -3518,11 +3659,12 @@
       <c r="J114" s="23"/>
       <c r="K114" s="17"/>
       <c r="L114" s="17"/>
-      <c r="M114" s="36"/>
-      <c r="N114" s="25"/>
-      <c r="O114" s="26"/>
-    </row>
-    <row r="115" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M114" s="17"/>
+      <c r="N114" s="36"/>
+      <c r="O114" s="25"/>
+      <c r="P114" s="26"/>
+    </row>
+    <row r="115" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A115" s="17"/>
       <c r="B115" s="34"/>
       <c r="C115" s="35"/>
@@ -3535,11 +3677,12 @@
       <c r="J115" s="23"/>
       <c r="K115" s="17"/>
       <c r="L115" s="17"/>
-      <c r="M115" s="36"/>
-      <c r="N115" s="25"/>
-      <c r="O115" s="26"/>
-    </row>
-    <row r="116" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M115" s="17"/>
+      <c r="N115" s="36"/>
+      <c r="O115" s="25"/>
+      <c r="P115" s="26"/>
+    </row>
+    <row r="116" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A116" s="17"/>
       <c r="B116" s="34"/>
       <c r="C116" s="35"/>
@@ -3552,11 +3695,12 @@
       <c r="J116" s="23"/>
       <c r="K116" s="17"/>
       <c r="L116" s="17"/>
-      <c r="M116" s="36"/>
-      <c r="N116" s="25"/>
-      <c r="O116" s="26"/>
-    </row>
-    <row r="117" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M116" s="17"/>
+      <c r="N116" s="36"/>
+      <c r="O116" s="25"/>
+      <c r="P116" s="26"/>
+    </row>
+    <row r="117" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A117" s="17"/>
       <c r="B117" s="34"/>
       <c r="C117" s="35"/>
@@ -3569,11 +3713,12 @@
       <c r="J117" s="23"/>
       <c r="K117" s="17"/>
       <c r="L117" s="17"/>
-      <c r="M117" s="36"/>
-      <c r="N117" s="25"/>
-      <c r="O117" s="26"/>
-    </row>
-    <row r="118" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="M117" s="17"/>
+      <c r="N117" s="36"/>
+      <c r="O117" s="25"/>
+      <c r="P117" s="26"/>
+    </row>
+    <row r="118" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A118" s="17"/>
       <c r="B118" s="34"/>
       <c r="C118" s="35"/>
@@ -3581,11 +3726,11 @@
       <c r="I118" s="22"/>
       <c r="J118" s="23"/>
       <c r="K118" s="17"/>
-      <c r="M118" s="36"/>
-      <c r="N118" s="25"/>
-      <c r="O118" s="26"/>
-    </row>
-    <row r="119" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N118" s="36"/>
+      <c r="O118" s="25"/>
+      <c r="P118" s="26"/>
+    </row>
+    <row r="119" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A119" s="17"/>
       <c r="B119" s="34"/>
       <c r="C119" s="35"/>
@@ -3593,11 +3738,11 @@
       <c r="I119" s="22"/>
       <c r="J119" s="23"/>
       <c r="K119" s="17"/>
-      <c r="M119" s="36"/>
-      <c r="N119" s="25"/>
-      <c r="O119" s="26"/>
-    </row>
-    <row r="120" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N119" s="36"/>
+      <c r="O119" s="25"/>
+      <c r="P119" s="26"/>
+    </row>
+    <row r="120" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A120" s="17"/>
       <c r="B120" s="34"/>
       <c r="C120" s="35"/>
@@ -3605,11 +3750,11 @@
       <c r="I120" s="22"/>
       <c r="J120" s="23"/>
       <c r="K120" s="17"/>
-      <c r="M120" s="36"/>
-      <c r="N120" s="25"/>
-      <c r="O120" s="26"/>
-    </row>
-    <row r="121" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N120" s="36"/>
+      <c r="O120" s="25"/>
+      <c r="P120" s="26"/>
+    </row>
+    <row r="121" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A121" s="17"/>
       <c r="B121" s="34"/>
       <c r="C121" s="35"/>
@@ -3617,11 +3762,11 @@
       <c r="I121" s="22"/>
       <c r="J121" s="23"/>
       <c r="K121" s="17"/>
-      <c r="M121" s="36"/>
-      <c r="N121" s="25"/>
-      <c r="O121" s="26"/>
-    </row>
-    <row r="122" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N121" s="36"/>
+      <c r="O121" s="25"/>
+      <c r="P121" s="26"/>
+    </row>
+    <row r="122" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A122" s="17"/>
       <c r="B122" s="34"/>
       <c r="C122" s="35"/>
@@ -3629,11 +3774,11 @@
       <c r="I122" s="22"/>
       <c r="J122" s="23"/>
       <c r="K122" s="17"/>
-      <c r="M122" s="36"/>
-      <c r="N122" s="25"/>
-      <c r="O122" s="26"/>
-    </row>
-    <row r="123" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N122" s="36"/>
+      <c r="O122" s="25"/>
+      <c r="P122" s="26"/>
+    </row>
+    <row r="123" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A123" s="17"/>
       <c r="B123" s="34"/>
       <c r="C123" s="35"/>
@@ -3641,11 +3786,11 @@
       <c r="I123" s="22"/>
       <c r="J123" s="23"/>
       <c r="K123" s="17"/>
-      <c r="M123" s="36"/>
-      <c r="N123" s="25"/>
-      <c r="O123" s="26"/>
-    </row>
-    <row r="124" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N123" s="36"/>
+      <c r="O123" s="25"/>
+      <c r="P123" s="26"/>
+    </row>
+    <row r="124" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A124" s="17"/>
       <c r="B124" s="34"/>
       <c r="C124" s="35"/>
@@ -3653,11 +3798,11 @@
       <c r="I124" s="22"/>
       <c r="J124" s="23"/>
       <c r="K124" s="17"/>
-      <c r="M124" s="36"/>
-      <c r="N124" s="25"/>
-      <c r="O124" s="26"/>
-    </row>
-    <row r="125" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N124" s="36"/>
+      <c r="O124" s="25"/>
+      <c r="P124" s="26"/>
+    </row>
+    <row r="125" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A125" s="17"/>
       <c r="B125" s="34"/>
       <c r="C125" s="35"/>
@@ -3665,11 +3810,11 @@
       <c r="I125" s="22"/>
       <c r="J125" s="23"/>
       <c r="K125" s="17"/>
-      <c r="M125" s="36"/>
-      <c r="N125" s="25"/>
-      <c r="O125" s="26"/>
-    </row>
-    <row r="126" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N125" s="36"/>
+      <c r="O125" s="25"/>
+      <c r="P125" s="26"/>
+    </row>
+    <row r="126" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A126" s="17"/>
       <c r="B126" s="34"/>
       <c r="C126" s="35"/>
@@ -3677,11 +3822,11 @@
       <c r="I126" s="22"/>
       <c r="J126" s="23"/>
       <c r="K126" s="17"/>
-      <c r="M126" s="36"/>
-      <c r="N126" s="25"/>
-      <c r="O126" s="26"/>
-    </row>
-    <row r="127" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N126" s="36"/>
+      <c r="O126" s="25"/>
+      <c r="P126" s="26"/>
+    </row>
+    <row r="127" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A127" s="17"/>
       <c r="B127" s="34"/>
       <c r="C127" s="35"/>
@@ -3689,11 +3834,11 @@
       <c r="I127" s="22"/>
       <c r="J127" s="23"/>
       <c r="K127" s="17"/>
-      <c r="M127" s="36"/>
-      <c r="N127" s="25"/>
-      <c r="O127" s="26"/>
-    </row>
-    <row r="128" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N127" s="36"/>
+      <c r="O127" s="25"/>
+      <c r="P127" s="26"/>
+    </row>
+    <row r="128" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A128" s="17"/>
       <c r="B128" s="34"/>
       <c r="C128" s="35"/>
@@ -3701,11 +3846,11 @@
       <c r="I128" s="22"/>
       <c r="J128" s="23"/>
       <c r="K128" s="17"/>
-      <c r="M128" s="36"/>
-      <c r="N128" s="25"/>
-      <c r="O128" s="26"/>
-    </row>
-    <row r="129" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N128" s="36"/>
+      <c r="O128" s="25"/>
+      <c r="P128" s="26"/>
+    </row>
+    <row r="129" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A129" s="17"/>
       <c r="B129" s="34"/>
       <c r="C129" s="35"/>
@@ -3713,11 +3858,11 @@
       <c r="I129" s="22"/>
       <c r="J129" s="23"/>
       <c r="K129" s="17"/>
-      <c r="M129" s="36"/>
-      <c r="N129" s="25"/>
-      <c r="O129" s="26"/>
-    </row>
-    <row r="130" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N129" s="36"/>
+      <c r="O129" s="25"/>
+      <c r="P129" s="26"/>
+    </row>
+    <row r="130" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A130" s="17"/>
       <c r="B130" s="34"/>
       <c r="C130" s="35"/>
@@ -3725,11 +3870,11 @@
       <c r="I130" s="22"/>
       <c r="J130" s="23"/>
       <c r="K130" s="17"/>
-      <c r="M130" s="36"/>
-      <c r="N130" s="25"/>
-      <c r="O130" s="26"/>
-    </row>
-    <row r="131" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N130" s="36"/>
+      <c r="O130" s="25"/>
+      <c r="P130" s="26"/>
+    </row>
+    <row r="131" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A131" s="17"/>
       <c r="B131" s="34"/>
       <c r="C131" s="35"/>
@@ -3737,11 +3882,11 @@
       <c r="I131" s="22"/>
       <c r="J131" s="23"/>
       <c r="K131" s="17"/>
-      <c r="M131" s="36"/>
-      <c r="N131" s="25"/>
-      <c r="O131" s="26"/>
-    </row>
-    <row r="132" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N131" s="36"/>
+      <c r="O131" s="25"/>
+      <c r="P131" s="26"/>
+    </row>
+    <row r="132" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A132" s="17"/>
       <c r="B132" s="34"/>
       <c r="C132" s="35"/>
@@ -3749,11 +3894,11 @@
       <c r="I132" s="22"/>
       <c r="J132" s="23"/>
       <c r="K132" s="17"/>
-      <c r="M132" s="36"/>
-      <c r="N132" s="25"/>
-      <c r="O132" s="26"/>
-    </row>
-    <row r="133" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N132" s="36"/>
+      <c r="O132" s="25"/>
+      <c r="P132" s="26"/>
+    </row>
+    <row r="133" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A133" s="17"/>
       <c r="B133" s="34"/>
       <c r="C133" s="35"/>
@@ -3761,11 +3906,11 @@
       <c r="I133" s="22"/>
       <c r="J133" s="23"/>
       <c r="K133" s="17"/>
-      <c r="M133" s="36"/>
-      <c r="N133" s="25"/>
-      <c r="O133" s="26"/>
-    </row>
-    <row r="134" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N133" s="36"/>
+      <c r="O133" s="25"/>
+      <c r="P133" s="26"/>
+    </row>
+    <row r="134" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A134" s="17"/>
       <c r="B134" s="34"/>
       <c r="C134" s="35"/>
@@ -3773,11 +3918,11 @@
       <c r="I134" s="22"/>
       <c r="J134" s="23"/>
       <c r="K134" s="17"/>
-      <c r="M134" s="36"/>
-      <c r="N134" s="25"/>
-      <c r="O134" s="26"/>
-    </row>
-    <row r="135" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N134" s="36"/>
+      <c r="O134" s="25"/>
+      <c r="P134" s="26"/>
+    </row>
+    <row r="135" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A135" s="17"/>
       <c r="B135" s="34"/>
       <c r="C135" s="35"/>
@@ -3785,11 +3930,11 @@
       <c r="I135" s="22"/>
       <c r="J135" s="23"/>
       <c r="K135" s="17"/>
-      <c r="M135" s="36"/>
-      <c r="N135" s="25"/>
-      <c r="O135" s="26"/>
-    </row>
-    <row r="136" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N135" s="36"/>
+      <c r="O135" s="25"/>
+      <c r="P135" s="26"/>
+    </row>
+    <row r="136" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A136" s="17"/>
       <c r="B136" s="34"/>
       <c r="C136" s="35"/>
@@ -3797,11 +3942,11 @@
       <c r="I136" s="22"/>
       <c r="J136" s="23"/>
       <c r="K136" s="17"/>
-      <c r="M136" s="36"/>
-      <c r="N136" s="25"/>
-      <c r="O136" s="26"/>
-    </row>
-    <row r="137" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N136" s="36"/>
+      <c r="O136" s="25"/>
+      <c r="P136" s="26"/>
+    </row>
+    <row r="137" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A137" s="17"/>
       <c r="B137" s="34"/>
       <c r="C137" s="35"/>
@@ -3809,11 +3954,11 @@
       <c r="I137" s="22"/>
       <c r="J137" s="23"/>
       <c r="K137" s="17"/>
-      <c r="M137" s="36"/>
-      <c r="N137" s="25"/>
-      <c r="O137" s="26"/>
-    </row>
-    <row r="138" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+      <c r="N137" s="36"/>
+      <c r="O137" s="25"/>
+      <c r="P137" s="26"/>
+    </row>
+    <row r="138" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A138" s="17"/>
       <c r="B138" s="34"/>
       <c r="C138" s="35"/>
@@ -3821,12 +3966,12 @@
       <c r="I138" s="22"/>
       <c r="J138" s="23"/>
       <c r="K138" s="17"/>
-      <c r="M138" s="36"/>
-      <c r="N138" s="25"/>
-      <c r="O138" s="26"/>
+      <c r="N138" s="36"/>
+      <c r="O138" s="25"/>
+      <c r="P138" s="26"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O138" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:P138" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <dataValidations count="6">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Classement produit" prompt="Veuillez saisir un chiffre supérieur ou égale à 1" sqref="A5:A1117" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
@@ -3840,15 +3985,15 @@
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Colisage" prompt="Veuillez saisir un chiffre supérieur ou égale à 1" sqref="K5:K1117" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Colisage" prompt="Veuillez saisir un chiffre supérieur ou égale à 1" sqref="K5:L1117" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L1117" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5:M1117" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5:N6 M7:M138 N8:N138 M139:N1117" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5:O6 N7:N138 O8:O138 N139:O1117" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>